<commit_message>
corpus hechos para iniciativas y audiencias, primeras comparaciones hechas
</commit_message>
<xml_diff>
--- a/entrada/iniciativas_ddff.xlsx
+++ b/entrada/iniciativas_ddff.xlsx
@@ -125,7 +125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="251">
   <si>
     <t xml:space="preserve">n</t>
   </si>
@@ -142,7 +142,7 @@
     <t xml:space="preserve">apoyos</t>
   </si>
   <si>
-    <t xml:space="preserve">texto_completo</t>
+    <t xml:space="preserve">texto</t>
   </si>
   <si>
     <t xml:space="preserve">solicito_ap</t>
@@ -1028,9 +1028,6 @@
 Coordinadora Feminista 8M (CF8M), Red Chilena contra la Violencia hacia las Mujeres, Asociación de Abogadas Feministas (Abofem), Agrupación de Familiares de Víctimas de Femicidios, Ni Una Menos Chile, Red de Actrices de Chile (RACH), Agrupación Lésbica Rompiendo el Silencio, Colectiva Feminista Patiperras La Serena, Manos que educan, Acción feminista Ovalle, Coordinadora feminista Illapel, Asamblea feminista Elki, ONG Educación y Comunicaciones (ECO), Comisión de género del Sindicato de Actrices y Actores de Chile (Sidarte), Graffitodas, Observatorio Equidad y Género, Movimiento por el Agua y Territorio, Organizando Trans Diversidades (OTD Chile), Comité Niñez y DDHH de CF8M, Aula Matemática y Género, Colectivo Cultura Popular La Escuela, Cooperativa la Cacerola de Ñuñoa, Asamblea Permanente por el Aborto, Escuela de Derecho Diurno de la Universidad Academia de Humanismo Cristiano, Frente feminista de Revolución Democrática, Asamblea de Mujeres San Borja-Yungay, PAQUENU+, Red de Filósofas Feministas, Colectiva Trenzas Sueltas, Colectiva Inkieta, Red Docente Feminista (Redofem) Libertadoras, Colectiva Mujeres Navidad, Colectiva mujeres libres de Pichilemu, Feministas Santa Cruz, Colectiva en movimiento mujeres y disidencias de Navidad, Movimiento de Defensa por el acceso al Agua, la Tierra y la Protección del Medio Ambiente (Modatima), Mujeres Wallmapu, CF8M Angol, Colectiva Llankanewen de Victoria, Asamblea feminista Yaneken de Galvarino y Agrupación Unión Sororas Licanray, además de mujeres y disidencias sexo genéricas autónomas</t>
   </si>
   <si>
-    <t xml:space="preserve">406, 408, 410, 310</t>
-  </si>
-  <si>
     <t xml:space="preserve">Los Primeros Mil Días: por el Derecho a la Protección de la Primera Infancia, la Maternidad y la Co-Parentalidad</t>
   </si>
   <si>
@@ -1077,9 +1074,6 @@
 Desde esta mesa de trabajo redactamos una carta al ministro de salud, que en pocos días contó con más 46.000 firmas de apoyo, y logramos la extensión del Postnatal De Emergencia trabajando en conjunto con diputadas y senadoras unidas transversalmente, más allá de sus diferencias y militancias políticas, juntas en apoyo a esta causa.
 Esta iniciativa de norma Constitucional nace desde el propósito mayor que nos reúne, desde el entendimiento de que la maternidad y la infancia no es sólo un asunto de madres. Es un asunto del futuro de toda nuestra sociedad y del Chile más digno que queremos construir.
 Sabemos que posicionar a las madres e infancias al centro de los cuidados sociales es la mejor forma de fortalecer a un pueblo que cuida y fortalece la calidad de vida de la ciudadanía desde el comienzo de la vida.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">204, 205</t>
   </si>
   <si>
     <t xml:space="preserve">Derechos de Niños, Niñas y Adolescentes reconocidos y consagrados en la nueva Constitución Política de la República</t>
@@ -1466,9 +1460,6 @@
 BREVE RESEÑA SOBRE QUIÉN O QUIÉNES PROPONEN Y LA HISTORIA DE LA ELABORACIÓN DE LA INICIATIVA
 Disidencias Unidas Recomponiendo Alianzas Sexopolíticas (D.U.R.A.S.) es una articulación de más de 42 organizaciones, colectivos y movimientos LGBTIQ+ de 9 regiones del país más 76 personas autocoonvocadas con el objetivo de incidir en la Convención Constitucional y su misión de redactar una nueva Constitución Política de la República que incorpore perspectivas de género transfeministas, que visibilice a las comunidades LGBTIQA(NB)+ y promueva su inclusión y no discriminación en el ejercicio de sus derechos.
 La elaboración de esta propuesta se hizo de manera ampliamente articulada teniendo como elemento rector, responder a las problemáticas en torno a las vejaciones y ejercicio de derechos que hemos tenido históricamente como población. En concreto generamos instancias de trabajo donde como representantes de los movimientos que componen DURAS, más el apoyo técnico de al menos 10 abogades con vasta experiencia en temas de diversidad y derechos, pudimos llegar a la síntesis del articulado que acá les presentamos. No está demás mencionar que nuestra propuesta pasó por varias instancias de observación tanto de profesionales del derecho, como por otres profesionales, personas comunes y corrientes, asesores constituyentes y convencionales constituyentes.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N.A</t>
   </si>
   <si>
     <t xml:space="preserve">Derecho a la identidad</t>
@@ -1882,9 +1873,6 @@
 La inciativa proviene del cuestionamiento sobre los derechos individuales en Chile e investigación sobre experiencias de personas que han tenido el derecho a elegir una muerte digna donde las mismas han corroborado que se sienten alividas de poder tener este esta opción y derecho.</t>
   </si>
   <si>
-    <t xml:space="preserve">N.A.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Derecho a la Alimentación, un Derecho Fundamental e Inalienable de los Pueblos</t>
   </si>
   <si>
@@ -2156,9 +2144,6 @@
 13. Asociación de Familiares y Amigos de Prematuros (ASFAPREM)
 14. Fundación Ciudadanía Inteligente (FCI)
 15. The Center for Economic and Social Rights (CESCR)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">¿108?</t>
   </si>
   <si>
     <t xml:space="preserve">Derecho a ser Club y ser Hincha</t>
@@ -2521,9 +2506,6 @@
 ciudad de Antofagasta y simultáneamente vía virtual, con más de 90 participantes, todos representantes o asesores de organizaciones sindicales.
 El tercer encuentro se realizó en la ciudad de Valparaíso el día 6 de noviembre pasado, también con conexión virtual, en el que se avanzó sobre la síntesis del Segundo Encuentro y se definieron y consensuaron precisiones respecto de la propuesta del Eje Sindical Constituyente. Contó con la participación de más de 60 dirigentes y la presencia de 5 constituyentes: Alondra Carrillo, Janis Meneses, Lissette Vergara, Dayyana González y María Rivera.
 En estas instancias hemos conocido las necesidades e inquietudes de trabajadoras y trabajadores, como asimismo de candidatos a convencionales, convencionales, asesores sindicales y académicos del Derecho del Trabajo, quienes nos han entregado su visión y aporte para la construcción de la presente propuesta.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">203/205</t>
   </si>
   <si>
     <t xml:space="preserve">Derecho a la Reinserción Social</t>
@@ -3197,12 +3179,12 @@
   <dimension ref="A1:AD1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.44"/>
@@ -4137,8 +4119,8 @@
       <c r="H19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I19" s="4" t="s">
-        <v>81</v>
+      <c r="I19" s="4" t="n">
+        <v>406</v>
       </c>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
@@ -4167,19 +4149,19 @@
         <v>56422</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="E20" s="3" t="n">
         <v>19108</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G20" s="2" t="n">
         <v>0</v>
@@ -4187,8 +4169,8 @@
       <c r="H20" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I20" s="4" t="s">
-        <v>86</v>
+      <c r="I20" s="4" t="n">
+        <v>405</v>
       </c>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
@@ -4217,19 +4199,19 @@
         <v>11402</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="E21" s="3" t="n">
         <v>18949</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G21" s="2" t="n">
         <v>0</v>
@@ -4267,19 +4249,19 @@
         <v>18394</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="E22" s="3" t="n">
         <v>18719</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G22" s="2" t="n">
         <v>1</v>
@@ -4317,19 +4299,19 @@
         <v>874</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="E23" s="3" t="n">
         <v>18474</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G23" s="2" t="n">
         <v>0</v>
@@ -4367,19 +4349,19 @@
         <v>43926</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="E24" s="3" t="n">
         <v>18467</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G24" s="2" t="n">
         <v>1</v>
@@ -4417,19 +4399,19 @@
         <v>57970</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="E25" s="3" t="n">
         <v>18282</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G25" s="2" t="n">
         <v>1</v>
@@ -4441,7 +4423,7 @@
         <v>311</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
@@ -4469,19 +4451,19 @@
         <v>6470</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="E26" s="3" t="n">
         <v>18255</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G26" s="2" t="n">
         <v>1</v>
@@ -4519,19 +4501,19 @@
         <v>45570</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="E27" s="3" t="n">
         <v>18065</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G27" s="2" t="n">
         <v>0</v>
@@ -4569,19 +4551,19 @@
         <v>10234</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>118</v>
       </c>
       <c r="E28" s="3" t="n">
         <v>18058</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G28" s="2" t="n">
         <v>1</v>
@@ -4589,11 +4571,11 @@
       <c r="H28" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I28" s="4" t="s">
-        <v>120</v>
+      <c r="I28" s="4" t="n">
+        <v>318</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
@@ -4621,19 +4603,19 @@
         <v>71122</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E29" s="3" t="n">
         <v>17964</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G29" s="2" t="n">
         <v>0</v>
@@ -4671,19 +4653,19 @@
         <v>43538</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E30" s="3" t="n">
         <v>17928</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G30" s="2" t="n">
         <v>0</v>
@@ -4721,19 +4703,19 @@
         <v>2826</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E31" s="3" t="n">
         <v>17495</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="G31" s="2" t="n">
         <v>1</v>
@@ -4771,19 +4753,19 @@
         <v>7062</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E32" s="3" t="n">
         <v>17294</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G32" s="2" t="n">
         <v>1</v>
@@ -4821,19 +4803,19 @@
         <v>3006</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E33" s="3" t="n">
         <v>17169</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G33" s="2" t="n">
         <v>0</v>
@@ -4871,19 +4853,19 @@
         <v>57370</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E34" s="3" t="n">
         <v>17087</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="G34" s="2" t="n">
         <v>0</v>
@@ -4921,19 +4903,19 @@
         <v>48926</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E35" s="3" t="n">
         <v>17001</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G35" s="2" t="n">
         <v>0</v>
@@ -4971,19 +4953,19 @@
         <v>73838</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E36" s="3" t="n">
         <v>16944</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G36" s="2" t="n">
         <v>0</v>
@@ -5021,19 +5003,19 @@
         <v>59750</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E37" s="3" t="n">
         <v>16891</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G37" s="2" t="n">
         <v>1</v>
@@ -5071,19 +5053,19 @@
         <v>4738</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E38" s="3" t="n">
         <v>16828</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G38" s="2" t="n">
         <v>1</v>
@@ -5121,19 +5103,19 @@
         <v>14698</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E39" s="3" t="n">
         <v>16652</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G39" s="2" t="n">
         <v>0</v>
@@ -5141,8 +5123,8 @@
       <c r="H39" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I39" s="4" t="s">
-        <v>166</v>
+      <c r="I39" s="4" t="n">
+        <v>309</v>
       </c>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
@@ -5171,19 +5153,19 @@
         <v>17046</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E40" s="3" t="n">
         <v>16641</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="G40" s="2" t="n">
         <v>1</v>
@@ -5221,19 +5203,19 @@
         <v>4126</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E41" s="3" t="n">
         <v>16460</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="G41" s="2" t="n">
         <v>1</v>
@@ -5271,19 +5253,19 @@
         <v>70062</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E42" s="3" t="n">
         <v>16459</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="G42" s="2" t="n">
         <v>1</v>
@@ -5321,19 +5303,19 @@
         <v>8082</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E43" s="3" t="n">
         <v>16444</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="G43" s="2" t="n">
         <v>1</v>
@@ -5371,19 +5353,19 @@
         <v>18202</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E44" s="3" t="n">
         <v>16388</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="G44" s="2" t="n">
         <v>1</v>
@@ -5391,8 +5373,8 @@
       <c r="H44" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I44" s="4" t="s">
-        <v>187</v>
+      <c r="I44" s="4" t="n">
+        <v>200</v>
       </c>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
@@ -5421,19 +5403,19 @@
         <v>11050</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="E45" s="3" t="n">
         <v>16155</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="G45" s="2" t="n">
         <v>1</v>
@@ -5471,19 +5453,19 @@
         <v>9638</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="E46" s="3" t="n">
         <v>16128</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="G46" s="2" t="n">
         <v>1</v>
@@ -5521,19 +5503,19 @@
         <v>45166</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="E47" s="3" t="n">
         <v>15558</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="G47" s="2" t="n">
         <v>1</v>
@@ -5571,19 +5553,19 @@
         <v>76538</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="E48" s="3" t="n">
         <v>12936</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="G48" s="2" t="n">
         <v>0</v>
@@ -5621,19 +5603,19 @@
         <v>10230</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E49" s="3" t="n">
         <v>10389</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="G49" s="2" t="n">
         <v>1</v>
@@ -5671,19 +5653,19 @@
         <v>46418</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E50" s="3" t="n">
         <v>8784</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="G50" s="2" t="n">
         <v>0</v>
@@ -5721,19 +5703,19 @@
         <v>61678</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="E51" s="3" t="n">
         <v>8225</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="G51" s="2" t="n">
         <v>1</v>
@@ -5771,19 +5753,19 @@
         <v>41706</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E52" s="3" t="n">
         <v>8061</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="G52" s="2" t="n">
         <v>1</v>
@@ -5821,19 +5803,19 @@
         <v>5614</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="E53" s="3" t="n">
         <v>7887</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="G53" s="2" t="n">
         <v>1</v>
@@ -5841,8 +5823,8 @@
       <c r="H53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I53" s="4" t="s">
-        <v>223</v>
+      <c r="I53" s="4" t="n">
+        <v>205</v>
       </c>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
@@ -5871,19 +5853,19 @@
         <v>66</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="E54" s="3" t="n">
         <v>7726</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G54" s="2" t="n">
         <v>1</v>
@@ -5921,19 +5903,19 @@
         <v>2458</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="E55" s="3" t="n">
         <v>7511</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G55" s="2" t="n">
         <v>0</v>
@@ -5971,19 +5953,19 @@
         <v>59370</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E56" s="3" t="n">
         <v>6026</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="G56" s="2" t="n">
         <v>0</v>
@@ -6021,19 +6003,19 @@
         <v>69382</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="E57" s="3" t="n">
         <v>6018</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="G57" s="2" t="n">
         <v>0</v>
@@ -6071,19 +6053,19 @@
         <v>50286</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="E58" s="3" t="n">
         <v>6005</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="G58" s="2" t="n">
         <v>1</v>
@@ -6121,19 +6103,19 @@
         <v>47390</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="E59" s="3" t="n">
         <v>5931</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="G59" s="2" t="n">
         <v>0</v>
@@ -6141,11 +6123,11 @@
       <c r="H59" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I59" s="4" t="s">
-        <v>166</v>
+      <c r="I59" s="4" t="n">
+        <v>413</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
@@ -6173,19 +6155,19 @@
         <v>11906</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="E60" s="3" t="n">
         <v>5794</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="G60" s="2" t="n">
         <v>1</v>
@@ -6223,19 +6205,19 @@
         <v>10074</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="E61" s="3" t="n">
         <v>5696</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="G61" s="2" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
correcciones de datos fuente
</commit_message>
<xml_diff>
--- a/entrada/iniciativas_ddff.xlsx
+++ b/entrada/iniciativas_ddff.xlsx
@@ -3179,12 +3179,12 @@
   <dimension ref="A1:AD1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.44"/>
@@ -3770,7 +3770,7 @@
         <v>0</v>
       </c>
       <c r="I12" s="4" t="n">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -4170,7 +4170,7 @@
         <v>0</v>
       </c>
       <c r="I20" s="4" t="n">
-        <v>405</v>
+        <v>410</v>
       </c>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
@@ -5124,7 +5124,7 @@
         <v>0</v>
       </c>
       <c r="I39" s="4" t="n">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>

</xml_diff>

<commit_message>
arreglo de código sanchez y rios
</commit_message>
<xml_diff>
--- a/entrada/iniciativas_ddff.xlsx
+++ b/entrada/iniciativas_ddff.xlsx
@@ -3179,12 +3179,12 @@
   <dimension ref="A1:AD1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
+      <selection pane="bottomLeft" activeCell="E43" activeCellId="0" sqref="E43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.44"/>

</xml_diff>